<commit_message>
example of excel file created when the user click on generate report
</commit_message>
<xml_diff>
--- a/public/reports/Reporte.xlsx
+++ b/public/reports/Reporte.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Documento N°</t>
   </si>
@@ -37,42 +37,33 @@
     <t>¿Paciente con error?</t>
   </si>
   <si>
-    <t>100742450</t>
+    <t>1007441850</t>
   </si>
   <si>
     <t>CC</t>
   </si>
   <si>
+    <t>2021-10-12</t>
+  </si>
+  <si>
+    <t>2021-11-24 10:20:09</t>
+  </si>
+  <si>
+    <t>Yulian Adolfo</t>
+  </si>
+  <si>
+    <t>Rojas Gañan</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>10074418506434</t>
+  </si>
+  <si>
     <t>2021-11-05</t>
   </si>
   <si>
-    <t>2021-11-25 13:47:44</t>
-  </si>
-  <si>
-    <t>asdlfkj</t>
-  </si>
-  <si>
-    <t>alsdkfj</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>1007441243</t>
-  </si>
-  <si>
-    <t>2021-11-25 13:37:37</t>
-  </si>
-  <si>
-    <t>asdflk</t>
-  </si>
-  <si>
-    <t>asdlkfj</t>
-  </si>
-  <si>
-    <t>10074418506434</t>
-  </si>
-  <si>
     <t>2021-11-25 13:48:44</t>
   </si>
   <si>
@@ -80,45 +71,6 @@
   </si>
   <si>
     <t>lasdkasfj</t>
-  </si>
-  <si>
-    <t>1007441345</t>
-  </si>
-  <si>
-    <t>2021-11-11</t>
-  </si>
-  <si>
-    <t>2021-11-27 19:20:45</t>
-  </si>
-  <si>
-    <t>Yulian Adolfo</t>
-  </si>
-  <si>
-    <t>Rojas Gañan</t>
-  </si>
-  <si>
-    <t>123450</t>
-  </si>
-  <si>
-    <t>2021-11-28 20:18:42</t>
-  </si>
-  <si>
-    <t>kljkj</t>
-  </si>
-  <si>
-    <t>asasdlfkj</t>
-  </si>
-  <si>
-    <t>1234567</t>
-  </si>
-  <si>
-    <t>2021-11-27 19:29:43</t>
-  </si>
-  <si>
-    <t>dflsafkjasklfdaskdlf</t>
-  </si>
-  <si>
-    <t>aldkdjfkslafl</t>
   </si>
 </sst>
 </file>
@@ -531,110 +483,18 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>